<commit_message>
Fixed max score issue in webterv 2nd milestone spreadsheet
</commit_message>
<xml_diff>
--- a/teaching/webterv/webterv_merfoldko_02.xlsx
+++ b/teaching/webterv/webterv_merfoldko_02.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumentumok\egyetem\oktatas\webterv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumentumok\egyetem\website\cservZ.github.io\teaching\webterv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F781BF-4BA4-4E54-8A9C-27402AB8E77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F42A89F-7BFA-40BA-BDA7-BFA7F15FE1EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{31CCB5CF-C965-4819-B7B9-D81D0E49B7CE}"/>
   </bookViews>
@@ -772,27 +772,7 @@
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00CC5C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color auto="1"/>
@@ -1200,7 +1180,7 @@
   <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1291,7 +1271,7 @@
         <v>34</v>
       </c>
       <c r="G5" s="12">
-        <f>MIN(SUM(C28:C45), 45)</f>
+        <f>MIN(SUM(C28:C45), 65)</f>
         <v>0</v>
       </c>
       <c r="I5" s="23" t="s">
@@ -2232,32 +2212,32 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A4:D11">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="7" priority="10">
       <formula>$C4="igen"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="11">
+    <cfRule type="expression" dxfId="6" priority="11">
       <formula>$C4="nem"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:D25 A28:D45">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>AND($C14=0,NOT(ISBLANK($C14)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>$C14=VALUE(RIGHT($B14,2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>NOT(ISBLANK($C14))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND($C49=0,NOT(ISBLANK($C49)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$C49=VALUE(RIGHT($B49,2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>NOT(ISBLANK($C49))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>